<commit_message>
Saldo Classic...Non ho capito quali argomenti ti servono, per il momento fa tutto direttamente in excel
</commit_message>
<xml_diff>
--- a/contabilità/contabilità.xlsx
+++ b/contabilità/contabilità.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_FDBC738146AD83244EAEC7E9165F976699F9D398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_FDBC738146AD83244EAEC7E9165F976699F9D398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6FA2FED-42CA-4EEA-80E6-524725534406}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Entrate</t>
   </si>
   <si>
     <t>Uscite</t>
+  </si>
+  <si>
+    <t>Saldo</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -367,16 +370,24 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1200</v>
       </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>200</v>
+      </c>
+      <c r="C3">
+        <v>-200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunto controllo sulla colonna saldo
</commit_message>
<xml_diff>
--- a/contabilità/contabilità.xlsx
+++ b/contabilità/contabilità.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_FDBC738146AD83244EAEC7E9165F976699F9D398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678A1406-2132-40A0-87AE-CE55DD93CAC9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="6290" yWindow="0" windowWidth="9600" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Entrate</t>
   </si>
   <si>
     <t>Uscite</t>
   </si>
+  <si>
+    <t>Saldo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -73,7 +77,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -350,32 +354,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1200</v>
       </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>200</v>
+      </c>
+      <c r="C3">
+        <v>-200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunto filtro per eliminare la riga di saldo dato che le righe sono dinamiche, poi ho aggiunto il saldo e sostituito la terza colonna da saldo a differenza. Poi ho aggiunto il messaggio per l'utente col valore del saldo
</commit_message>
<xml_diff>
--- a/contabilità/contabilità.xlsx
+++ b/contabilità/contabilità.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_FDBC738146AD83244EAEC7E9165F976699F9D398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678A1406-2132-40A0-87AE-CE55DD93CAC9}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_FDBC738146AD83244EAEC7E9165F976699F9D398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{458D383E-3CC3-41FE-8F65-7FAE8CB74102}"/>
   <bookViews>
-    <workbookView xWindow="6290" yWindow="0" windowWidth="9600" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2750" yWindow="300" windowWidth="9600" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Entrate</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Saldo</t>
+  </si>
+  <si>
+    <t>Differenza</t>
   </si>
 </sst>
 </file>
@@ -355,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -371,7 +374,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -388,6 +391,25 @@
       </c>
       <c r="C3">
         <v>-200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3000</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>